<commit_message>
feat: enhance apostolate data processing and UI components
- Introduce a new function to safely retrieve and clean string values from Excel data.
- Update slugify function to handle special characters for apostolate names.
- Improve activity processing to differentiate between list and paragraph formats.
- Add truncation functionality for apostolate descriptions in the ApostolCard component.
- Implement list formatting in the ApostolModal for better display of activities.
- Add new apostolate data for Movimiento de Espiritualidad Matrimonial (MEM) and update existing entries with coordinator information and activities.
</commit_message>
<xml_diff>
--- a/Formulario de Apostolados_ Pagina Web (respuestas).xlsx
+++ b/Formulario de Apostolados_ Pagina Web (respuestas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -160,6 +160,81 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1ute_uXAOGHpSelniTRYJepI6AXcxjouP</t>
+  </si>
+  <si>
+    <t>mariobohorquezg@gmail.com</t>
+  </si>
+  <si>
+    <t>Movímiento de Espiritualidad Matrimonial (MEM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memmaracaibo </t>
+  </si>
+  <si>
+    <t>Fomentar la espiritualidad conyugal de los esposos y la santificación matrimonial a través de las actividades
+ordinarias. Ser un factor de gran influencia en nuestras familias y en la sociedad para impulsar la vocación
+matrimonial como célula de nuestra Iglesia.
+Proveer un espacio para que los matrimonios revivan el amor conyugal, teniendo a Cristo como centro de su
+alianza matrimonial a través de Retiros de Espiritualidad Matrimonial, la meditación de La Palabra, actividades
+de formación y apoyando las actividades de apostolado de la parroquia.</t>
+  </si>
+  <si>
+    <t>Este movimiento nació en octubre de 1990 cuando el Padre Antonio Abella, entonces párroco de la iglesia San
+Ramón Nonato, por inspiración divina conformó una serie de meditaciones sobre la vocación del matrimonio a
+la luz de la Palabra de Dios y realizó el primer Retiro de Espiritualidad Matrimonial (REM) a tres matrimonios de
+la parroquia.
+El retiro se diseñó con la finalidad de intensificar la doctrina matrimonial y fundamentar la espiritualidad de los
+esposos en la Palabra de Dios, mediante un conjunto de charlas, reflexiones, oraciones y celebraciones litúrgicas
+a las que se recurre durante cuarenta y ocho horas que dura el retiro.
+A partir del segundo retiro realizado en Maracaibo, el REM se constituyó como grupo parroquial, estableciéndose
+reuniones semanales como medio fundamental para acrecentar la fe, canalizar la formación y el crecimiento
+espiritual de los esposos. Posteriormente y junto a la realización de retiros periódicos y la participación de las
+parejas en actividades apostólicas de la parroquia, el grupo se dedicó a dictar los cursillos prematrimoniales y
+catequesis de niños y jóvenes.
+Luego de consolidarse el REM como grupo parroquial en la década de los años 90, por iniciativa del Padre Antonio
+Abella y con la aceptación y beneplácito de todos los matrimonios participantes, en octubre del 2000 el grupo
+pasó a llamarse Movimiento de Espiritualidad Matrimonial (MEM).
+La sucesión de la dirección espiritual del MEM en sentido cronológico desde su nacimiento, es como sigue:
+• P. Antonio Abella (1990-1996)
+• P. José Zaporta (1996-1998)
+• P. Francisco Ortiz (1998-2000)
+• P. Jesús García (2000-2003)
+• P. Néstor Burgos (2007-2009)
+• P. Jesús Bel (2009-2014)
+• P. Richard Godoy (2014 hasta el presente)
+Con el pasar del tiempo las actividades del REM fueron paulatinamente pasando al liderazgo de los propios
+matrimonios del movimiento quienes se han pasado el testigo manteniendo intactas las reflexiones originales
+del P. Antonio Abella, siempre con la guía espiritual del párroco de San Ramón Nonato y bajo el amparo y gracia
+del Espíritu Santo a quien consagramos con fervor nuestro movimiento y apostolado.
+Desde 2018 el MEM se constituyó como la sección “Adultos y Familia” de la Acción Católica de Venezuela y
+comenzó a realizar retiros de espiritualidad matrimonial dedicados a nuevas parroquias de Maracaibo,
+empezando por Santa Rosa de Lima y San Bartolomé Apóstol (Ziruma), para convertirse en una institución laical
+enfocada a la Pastoral Familiar, que tiene como principal apostolado la lucha por el fortalecimiento del
+matrimonio católico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mario Bohórquez de Fernández </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mónica Fernández de Bohorquez </t>
+  </si>
+  <si>
+    <t>04146178604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrimonios o parejas de unión libre en concubinato o parejas de divorciados y vueltos a casar </t>
+  </si>
+  <si>
+    <t>Miércoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:30 pm - 8:30 pm </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1EZ875Kc0bR40h4zJ1FqrcCJuoj9LQqYv</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Ag50xlJ6e4U5FaG71pOVC_KifmN2od49</t>
   </si>
 </sst>
 </file>
@@ -295,7 +370,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q3" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q4" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="17">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Dirección de correo electrónico" id="2"/>
@@ -704,16 +779,71 @@
         <v>47</v>
       </c>
     </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="2">
+        <v>46013.42023517361</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4.246144593E9</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="P2"/>
     <hyperlink r:id="rId2" ref="Q2"/>
     <hyperlink r:id="rId3" ref="P3"/>
     <hyperlink r:id="rId4" ref="Q3"/>
+    <hyperlink r:id="rId5" ref="P4"/>
+    <hyperlink r:id="rId6" ref="Q4"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update apostolate data and add new images
- Add new apostolate data for Jóvenes de Acción Católica Mercedaria, including detailed descriptions, activities, and coordinator information.
- Update existing apostolate entries with improved translations and image paths.
- Introduce new images for apostolates to enhance visual representation in the application.
- Modify chapel data structure to include the new apostolate and ensure consistency across translations.
</commit_message>
<xml_diff>
--- a/Formulario de Apostolados_ Pagina Web (respuestas).xlsx
+++ b/Formulario de Apostolados_ Pagina Web (respuestas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -235,6 +235,40 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1Ag50xlJ6e4U5FaG71pOVC_KifmN2od49</t>
+  </si>
+  <si>
+    <t>Jóvenes de Acción Católica Mercedaria</t>
+  </si>
+  <si>
+    <t>@jacm.sanramon</t>
+  </si>
+  <si>
+    <t>Pastoral Juvenil Parroquial adherida a los estatutos de la Acción Católica (asociación de laicos para laicos) y siguiendo el carisma Mercedario (carisma de la Parroquia)</t>
+  </si>
+  <si>
+    <t>- Encuentros Formativos: Espacios de formación para los jóvenes de la parroquia (pertenecientes al grupo e invitados)
+- Liturgia: Encargados de la liturgia de la Eucaristía de los Viernes a las 5:00 PM (previa a los encuentros)
+- Acción Social: Por los menos dos o tres acciones sociales trimestrales en los barrios pertenecientes a la comunidad
+- Experiencias Espirituales: Convivencias y retiros espirituales abiertos para jóvenes de la parroquia
+- JAC-MEM: Encuentros combinados con Pastoral Familiar como método de preparación para la generación de relevo</t>
+  </si>
+  <si>
+    <t>Victor Kneider</t>
+  </si>
+  <si>
+    <t>04246501227</t>
+  </si>
+  <si>
+    <t>Jóvenes</t>
+  </si>
+  <si>
+    <t>Viernes de 5 PM a 8 PM</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Tw8D3hctSFlOJIcZ7JQLBNhUrNlGPpea</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1LLWyeQkEfAM1vR32udBDK4_ija6gUjSg</t>
   </si>
 </sst>
 </file>
@@ -370,7 +404,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q4" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q5" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="17">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Dirección de correo electrónico" id="2"/>
@@ -832,6 +866,59 @@
         <v>60</v>
       </c>
     </row>
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="2">
+        <v>46013.561763125</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="P2"/>
@@ -840,10 +927,12 @@
     <hyperlink r:id="rId4" ref="Q3"/>
     <hyperlink r:id="rId5" ref="P4"/>
     <hyperlink r:id="rId6" ref="Q4"/>
+    <hyperlink r:id="rId7" ref="P5"/>
+    <hyperlink r:id="rId8" ref="Q5"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>